<commit_message>
API change on cellreader (loadcell only takes one test-set (resfiles must be given, if cellpyfile is given, check for updates compared to resfiles)
</commit_message>
<xml_diff>
--- a/cellpy/databases/cellpy_db.xlsx
+++ b/cellpy/databases/cellpy_db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="7410" windowWidth="24240" windowHeight="7215" tabRatio="376"/>
+    <workbookView xWindow="-15" yWindow="7410" windowWidth="24240" windowHeight="7215" tabRatio="376" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="db_table" sheetId="14" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="118">
   <si>
     <t>Sr.No</t>
   </si>
@@ -273,12 +273,6 @@
     <t>3_22</t>
   </si>
   <si>
-    <t>20140918_is021_01_cc</t>
-  </si>
-  <si>
-    <t>20140918_is021_01_cc_01.res</t>
-  </si>
-  <si>
     <t>20140918_is021_02_cc</t>
   </si>
   <si>
@@ -370,6 +364,15 @@
   </si>
   <si>
     <t>Fixed</t>
+  </si>
+  <si>
+    <t>20160805_test001_45_cc</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>20160805_test001_45_cc_01.res</t>
   </si>
 </sst>
 </file>
@@ -377,8 +380,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -465,15 +468,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -807,11 +810,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AV16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomRight" activeCell="S3" sqref="A3:S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1113,20 +1116,20 @@
         <v>45</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D3" s="24">
         <v>1</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="24" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
@@ -1137,13 +1140,13 @@
       </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="6" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="T3" s="6">
         <v>0</v>
@@ -1233,20 +1236,20 @@
         <v>45</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D4" s="24">
         <v>1</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
@@ -1257,13 +1260,13 @@
       </c>
       <c r="P4" s="7"/>
       <c r="Q4" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="T4" s="6">
         <v>0</v>
@@ -1353,20 +1356,20 @@
         <v>45</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D5" s="24">
         <v>1</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
@@ -1377,13 +1380,13 @@
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="T5" s="6">
         <v>0</v>
@@ -1473,20 +1476,20 @@
         <v>45</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" s="24">
         <v>1</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
@@ -1497,13 +1500,13 @@
       </c>
       <c r="P6" s="7"/>
       <c r="Q6" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="T6" s="6">
         <v>0</v>
@@ -1593,20 +1596,20 @@
         <v>45</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D7" s="24">
         <v>1</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
@@ -1617,13 +1620,13 @@
       </c>
       <c r="P7" s="7"/>
       <c r="Q7" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="T7" s="6">
         <v>0</v>
@@ -1713,20 +1716,20 @@
         <v>45</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D8" s="24">
         <v>1</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
@@ -1737,13 +1740,13 @@
       </c>
       <c r="P8" s="7"/>
       <c r="Q8" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="T8" s="6">
         <v>0</v>
@@ -1833,7 +1836,7 @@
         <v>45</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D9" s="24">
         <v>0</v>
@@ -1842,13 +1845,13 @@
         <v>67</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
@@ -1857,13 +1860,13 @@
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S9" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="T9" s="6">
         <v>0</v>
@@ -1953,20 +1956,20 @@
         <v>46</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D10" s="24">
         <v>1</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
@@ -1977,13 +1980,13 @@
       </c>
       <c r="P10" s="7"/>
       <c r="Q10" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="S10" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T10" s="6">
         <v>0</v>
@@ -2073,20 +2076,20 @@
         <v>46</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D11" s="24">
         <v>1</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
@@ -2097,13 +2100,13 @@
       </c>
       <c r="P11" s="7"/>
       <c r="Q11" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="S11" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T11" s="6">
         <v>0</v>
@@ -2193,20 +2196,20 @@
         <v>46</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D12" s="24">
         <v>1</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -2217,13 +2220,13 @@
       </c>
       <c r="P12" s="7"/>
       <c r="Q12" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="R12" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="S12" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T12" s="6">
         <v>0</v>
@@ -2313,20 +2316,20 @@
         <v>46</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D13" s="24">
         <v>1</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
@@ -2337,13 +2340,13 @@
       </c>
       <c r="P13" s="7"/>
       <c r="Q13" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T13" s="6">
         <v>0</v>
@@ -2433,20 +2436,20 @@
         <v>46</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D14" s="24">
         <v>1</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -2457,13 +2460,13 @@
       </c>
       <c r="P14" s="7"/>
       <c r="Q14" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="R14" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T14" s="6">
         <v>0</v>
@@ -2553,20 +2556,20 @@
         <v>46</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D15" s="24">
         <v>1</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
@@ -2577,13 +2580,13 @@
       </c>
       <c r="P15" s="7"/>
       <c r="Q15" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="R15" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T15" s="6">
         <v>0</v>
@@ -2673,7 +2676,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D16" s="24">
         <v>0</v>
@@ -2682,13 +2685,13 @@
         <v>67</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
@@ -2697,13 +2700,13 @@
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="S16" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T16" s="6">
         <v>0</v>
@@ -2796,9 +2799,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2831,11 +2834,12 @@
       <c r="A3">
         <v>614</v>
       </c>
-      <c r="B3" t="s">
-        <v>84</v>
+      <c r="B3" t="str">
+        <f>db_table!Q3</f>
+        <v>20160805_test001_45_cc</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -2843,10 +2847,10 @@
         <v>615</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -2854,10 +2858,10 @@
         <v>616</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -2865,10 +2869,10 @@
         <v>617</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -2876,10 +2880,10 @@
         <v>618</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -2887,10 +2891,10 @@
         <v>619</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -2898,7 +2902,7 @@
         <v>620</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -2906,10 +2910,10 @@
         <v>621</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -2917,10 +2921,10 @@
         <v>622</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -2928,10 +2932,10 @@
         <v>623</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -2939,10 +2943,10 @@
         <v>624</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -2950,10 +2954,10 @@
         <v>625</v>
       </c>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -2961,10 +2965,10 @@
         <v>626</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -2972,7 +2976,7 @@
         <v>627</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3223,18 +3227,18 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B23" s="3">
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adds dbreader filter on columns
</commit_message>
<xml_diff>
--- a/cellpy/databases/cellpy_db.xlsx
+++ b/cellpy/databases/cellpy_db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="7410" windowWidth="24240" windowHeight="7215" tabRatio="376" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="7410" windowWidth="24240" windowHeight="7215" tabRatio="376"/>
   </bookViews>
   <sheets>
     <sheet name="db_table" sheetId="14" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="121">
   <si>
     <t>Sr.No</t>
   </si>
@@ -373,6 +373,15 @@
   </si>
   <si>
     <t>20160805_test001_45_cc_01.res</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>VC</t>
+  </si>
+  <si>
+    <t>FEC</t>
   </si>
 </sst>
 </file>
@@ -810,11 +819,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AV16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S3" sqref="A3:S3"/>
+      <selection pane="bottomRight" activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -919,9 +928,15 @@
       <c r="T1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="6"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="6"/>
+      <c r="U1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="V1" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="X1" s="18"/>
       <c r="Y1" s="6"/>
       <c r="Z1" s="20"/>
@@ -1149,10 +1164,10 @@
         <v>116</v>
       </c>
       <c r="T3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3" s="22">
         <v>0</v>
@@ -1269,7 +1284,7 @@
         <v>110</v>
       </c>
       <c r="T4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" s="6">
         <v>0</v>
@@ -2799,7 +2814,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>

</xml_diff>

<commit_message>
adds many new tests for dbreader and cleans up the test files a little bit
</commit_message>
<xml_diff>
--- a/cellpy/databases/cellpy_db.xlsx
+++ b/cellpy/databases/cellpy_db.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="124">
   <si>
     <t>Sr.No</t>
   </si>
@@ -382,6 +382,15 @@
   </si>
   <si>
     <t>FEC</t>
+  </si>
+  <si>
+    <t>exp002</t>
+  </si>
+  <si>
+    <t>test comment general</t>
+  </si>
+  <si>
+    <t>28</t>
   </si>
 </sst>
 </file>
@@ -467,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -512,6 +521,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,20 +827,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AV16"/>
+  <dimension ref="A1:BE18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AK3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V9" sqref="V9"/>
+      <selection pane="bottomRight" activeCell="AN4" sqref="AN4:AN6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="17" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" style="25" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" style="25" customWidth="1"/>
@@ -840,7 +850,7 @@
     <col min="11" max="13" width="4.5703125" style="2" customWidth="1"/>
     <col min="14" max="14" width="6.5703125" style="2" customWidth="1"/>
     <col min="15" max="15" width="7" style="2" customWidth="1"/>
-    <col min="16" max="16" width="6.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="2" customWidth="1"/>
     <col min="17" max="17" width="23.5703125" customWidth="1"/>
     <col min="18" max="18" width="27.5703125" customWidth="1"/>
     <col min="19" max="19" width="59.28515625" customWidth="1"/>
@@ -858,12 +868,12 @@
     <col min="37" max="37" width="10" customWidth="1"/>
     <col min="38" max="38" width="13.85546875" customWidth="1"/>
     <col min="39" max="39" width="24.85546875" customWidth="1"/>
-    <col min="40" max="40" width="7.85546875" style="11" customWidth="1"/>
+    <col min="40" max="40" width="22" style="11" customWidth="1"/>
     <col min="41" max="41" width="9.140625" style="4" customWidth="1"/>
-    <col min="42" max="42" width="5.85546875" customWidth="1"/>
-    <col min="43" max="43" width="12.28515625" style="13" customWidth="1"/>
-    <col min="44" max="44" width="8.140625" style="13" customWidth="1"/>
-    <col min="45" max="47" width="8.140625" style="13" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="19.7109375" customWidth="1"/>
+    <col min="43" max="43" width="26.140625" style="13" customWidth="1"/>
+    <col min="44" max="44" width="18.28515625" style="13" customWidth="1"/>
+    <col min="45" max="47" width="8.140625" style="13" customWidth="1"/>
     <col min="48" max="48" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1149,7 +1159,9 @@
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
+      <c r="N3" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="O3" s="7" t="s">
         <v>29</v>
       </c>
@@ -1241,7 +1253,9 @@
       <c r="AS3" s="12"/>
       <c r="AT3" s="12"/>
       <c r="AU3" s="12"/>
-      <c r="AV3" s="6"/>
+      <c r="AV3" s="6" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="4" spans="1:48" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
@@ -1273,7 +1287,9 @@
       <c r="O4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="7"/>
+      <c r="P4" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="Q4" s="6" t="s">
         <v>84</v>
       </c>
@@ -1284,7 +1300,7 @@
         <v>110</v>
       </c>
       <c r="T4" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" s="6">
         <v>0</v>
@@ -1332,7 +1348,7 @@
         <v>69</v>
       </c>
       <c r="AJ4" s="8">
-        <v>0.45438760079739932</v>
+        <v>0.45438760079739898</v>
       </c>
       <c r="AK4" s="6" t="s">
         <v>21</v>
@@ -1971,7 +1987,7 @@
         <v>46</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D10" s="24">
         <v>1</v>
@@ -2091,7 +2107,7 @@
         <v>46</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D11" s="24">
         <v>1</v>
@@ -2211,7 +2227,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D12" s="24">
         <v>1</v>
@@ -2331,7 +2347,7 @@
         <v>46</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D13" s="24">
         <v>1</v>
@@ -2451,7 +2467,7 @@
         <v>46</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D14" s="24">
         <v>1</v>
@@ -2571,7 +2587,7 @@
         <v>46</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D15" s="24">
         <v>1</v>
@@ -2691,7 +2707,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D16" s="24">
         <v>0</v>
@@ -2802,6 +2818,231 @@
       <c r="AT16" s="12"/>
       <c r="AU16" s="12"/>
       <c r="AV16" s="6"/>
+    </row>
+    <row r="18" spans="1:57" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="28">
+        <f>1+B18</f>
+        <v>2</v>
+      </c>
+      <c r="D18" s="28">
+        <f t="shared" ref="D18:BB18" si="0">1+C18</f>
+        <v>3</v>
+      </c>
+      <c r="E18" s="28">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F18" s="28">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G18" s="28">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H18" s="28">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I18" s="28">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J18" s="28">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K18" s="28">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L18" s="28">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="M18" s="28">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="N18" s="28">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="O18" s="28">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="P18" s="28">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="Q18" s="28">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="R18" s="28">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="S18" s="28">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="T18" s="28">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="U18" s="28">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="V18" s="28">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="W18" s="28">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="X18" s="28">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="Y18" s="28">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="Z18" s="28">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AA18" s="28">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="AB18" s="28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AC18" s="28">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AD18" s="28">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="AE18" s="28">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AF18" s="28">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="AG18" s="28">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="AH18" s="28">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="AI18" s="28">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="AJ18" s="28">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="AK18" s="28">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="AL18" s="28">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="AM18" s="28">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="AN18" s="28">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="AO18" s="28">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="AP18" s="28">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="AQ18" s="28">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="AR18" s="28">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="AS18" s="28">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="AT18" s="28">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="AU18" s="28">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="AV18" s="28">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="AW18" s="28">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="AX18" s="28">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="AY18" s="28">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="AZ18" s="28">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="BA18" s="28">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="BB18" s="28">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="BC18" s="6">
+        <v>27</v>
+      </c>
+      <c r="BD18" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="BE18" s="6">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3004,8 +3245,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
tries first attempt to add logging
</commit_message>
<xml_diff>
--- a/cellpy/databases/cellpy_db.xlsx
+++ b/cellpy/databases/cellpy_db.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="123">
   <si>
     <t>Sr.No</t>
   </si>
@@ -388,9 +388,6 @@
   </si>
   <si>
     <t>test comment general</t>
-  </si>
-  <si>
-    <t>28</t>
   </si>
 </sst>
 </file>
@@ -830,10 +827,10 @@
   <dimension ref="A1:BE18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AK3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AN4" sqref="AN4:AN6"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2820,229 +2817,62 @@
       <c r="AV16" s="6"/>
     </row>
     <row r="18" spans="1:57" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>0</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="28">
-        <f>1+B18</f>
-        <v>2</v>
-      </c>
-      <c r="D18" s="28">
-        <f t="shared" ref="D18:BB18" si="0">1+C18</f>
-        <v>3</v>
-      </c>
-      <c r="E18" s="28">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F18" s="28">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="G18" s="28">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H18" s="28">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="I18" s="28">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="J18" s="28">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="K18" s="28">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L18" s="28">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="M18" s="28">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="N18" s="28">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="O18" s="28">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="P18" s="28">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="Q18" s="28">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="R18" s="28">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="S18" s="28">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="T18" s="28">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="U18" s="28">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="V18" s="28">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="W18" s="28">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="X18" s="28">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="Y18" s="28">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="Z18" s="28">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="AA18" s="28">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="AB18" s="28">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="AC18" s="28">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="AD18" s="28">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="AE18" s="28">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="AF18" s="28">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="AG18" s="28">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="AH18" s="28">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="AI18" s="28">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="AJ18" s="28">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="AK18" s="28">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="AL18" s="28">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="AM18" s="28">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="AN18" s="28">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="AO18" s="28">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="AP18" s="28">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="AQ18" s="28">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="AR18" s="28">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="AS18" s="28">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="AT18" s="28">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AU18" s="28">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="AV18" s="28">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="AW18" s="28">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="AX18" s="28">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="AY18" s="28">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="AZ18" s="28">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="BA18" s="28">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="BB18" s="28">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="BC18" s="6">
-        <v>27</v>
-      </c>
-      <c r="BD18" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="BE18" s="6">
-        <v>28</v>
-      </c>
+      <c r="A18" s="6"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="28"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="28"/>
+      <c r="X18" s="28"/>
+      <c r="Y18" s="28"/>
+      <c r="Z18" s="28"/>
+      <c r="AA18" s="28"/>
+      <c r="AB18" s="28"/>
+      <c r="AC18" s="28"/>
+      <c r="AD18" s="28"/>
+      <c r="AE18" s="28"/>
+      <c r="AF18" s="28"/>
+      <c r="AG18" s="28"/>
+      <c r="AH18" s="28"/>
+      <c r="AI18" s="28"/>
+      <c r="AJ18" s="28"/>
+      <c r="AK18" s="28"/>
+      <c r="AL18" s="28"/>
+      <c r="AM18" s="28"/>
+      <c r="AN18" s="28"/>
+      <c r="AO18" s="28"/>
+      <c r="AP18" s="28"/>
+      <c r="AQ18" s="28"/>
+      <c r="AR18" s="28"/>
+      <c r="AS18" s="28"/>
+      <c r="AT18" s="28"/>
+      <c r="AU18" s="28"/>
+      <c r="AV18" s="28"/>
+      <c r="AW18" s="28"/>
+      <c r="AX18" s="28"/>
+      <c r="AY18" s="28"/>
+      <c r="AZ18" s="28"/>
+      <c r="BA18" s="28"/>
+      <c r="BB18" s="28"/>
+      <c r="BC18" s="6"/>
+      <c r="BD18" s="2"/>
+      <c r="BE18" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>